<commit_message>
update shelmire planting spreadsheet
</commit_message>
<xml_diff>
--- a/src/xls/shelmire.xlsx
+++ b/src/xls/shelmire.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chirs/repos/planting/src/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332060D6-8485-7C4E-807B-134EEC309BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA413D0-DAAF-BF40-9DF0-61C844C858CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{15BA4F13-2581-9841-A9DF-6B3D6C84267C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="4" xr2:uid="{15BA4F13-2581-9841-A9DF-6B3D6C84267C}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="6" r:id="rId1"/>
     <sheet name="species" sheetId="1" r:id="rId2"/>
     <sheet name="x" sheetId="4" r:id="rId3"/>
-    <sheet name="seeds" sheetId="5" r:id="rId4"/>
-    <sheet name="families" sheetId="2" r:id="rId5"/>
-    <sheet name="references" sheetId="3" r:id="rId6"/>
+    <sheet name="families" sheetId="2" r:id="rId4"/>
+    <sheet name="references" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1916" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="718">
   <si>
     <t>Southern blackhaw</t>
   </si>
@@ -1957,12 +1956,357 @@
   <si>
     <t>Lantana camara</t>
   </si>
+  <si>
+    <t>Rosemarinus officinalis</t>
+  </si>
+  <si>
+    <t>Ilex crenata</t>
+  </si>
+  <si>
+    <t>Trachelospermum asiaticum</t>
+  </si>
+  <si>
+    <t>Nandina domestica</t>
+  </si>
+  <si>
+    <t>Ilex cornuta</t>
+  </si>
+  <si>
+    <t>Cynodon dactylon</t>
+  </si>
+  <si>
+    <t>Stenotaphrum secundatum</t>
+  </si>
+  <si>
+    <t>Broadleaf plantain</t>
+  </si>
+  <si>
+    <t>Plantago major</t>
+  </si>
+  <si>
+    <t>Gum bumelia</t>
+  </si>
+  <si>
+    <t>Sideroxylon lanuginosum</t>
+  </si>
+  <si>
+    <t>Spicebush</t>
+  </si>
+  <si>
+    <t>Lindera benzoin</t>
+  </si>
+  <si>
+    <t>Toothed spurge</t>
+  </si>
+  <si>
+    <t>Virginia pepperweed</t>
+  </si>
+  <si>
+    <t>Lepidium virginicum</t>
+  </si>
+  <si>
+    <t>Texas persimmon</t>
+  </si>
+  <si>
+    <t>American persimmon</t>
+  </si>
+  <si>
+    <t>Cotton morning glory</t>
+  </si>
+  <si>
+    <t>Ipomoea cordatotriloba</t>
+  </si>
+  <si>
+    <t>Carolina snailseed</t>
+  </si>
+  <si>
+    <t>Cocculus carolinus</t>
+  </si>
+  <si>
+    <t>Euphorbia dentata</t>
+  </si>
+  <si>
+    <t>White mulberry</t>
+  </si>
+  <si>
+    <t>Cynanchum laeve</t>
+  </si>
+  <si>
+    <t>Honeyvine milkweed</t>
+  </si>
+  <si>
+    <t>Diospyros texana</t>
+  </si>
+  <si>
+    <t>Diospyros virginiana</t>
+  </si>
+  <si>
+    <t>Lemon beebalm</t>
+  </si>
+  <si>
+    <t>Monarda citriodora</t>
+  </si>
+  <si>
+    <t>Texas kidneywood</t>
+  </si>
+  <si>
+    <t>Texas Kidneywood</t>
+  </si>
+  <si>
+    <t>Mustang grape</t>
+  </si>
+  <si>
+    <t>Vitis mustangensis</t>
+  </si>
+  <si>
+    <t>Partridge pea</t>
+  </si>
+  <si>
+    <t>Prairie goldenrod</t>
+  </si>
+  <si>
+    <t>Solidago missouriensis</t>
+  </si>
+  <si>
+    <t>Chamaecrista fasciculata</t>
+  </si>
+  <si>
+    <t>Tagetes lucida</t>
+  </si>
+  <si>
+    <t>Mexican tarragon</t>
+  </si>
+  <si>
+    <t>Black-eyed Susan</t>
+  </si>
+  <si>
+    <t>Rudbeckia hirta</t>
+  </si>
+  <si>
+    <t>regional</t>
+  </si>
+  <si>
+    <t>Carya glabra</t>
+  </si>
+  <si>
+    <t>Pignut hickory</t>
+  </si>
+  <si>
+    <t>Hibiscus coccineus</t>
+  </si>
+  <si>
+    <t>Texas star hibiscus</t>
+  </si>
+  <si>
+    <t>Senna lindheimeriana</t>
+  </si>
+  <si>
+    <t>Velvet leaf senna</t>
+  </si>
+  <si>
+    <t>Celtis occidentalis</t>
+  </si>
+  <si>
+    <t>Common hackberry</t>
+  </si>
+  <si>
+    <t>Morus alba</t>
+  </si>
+  <si>
+    <t>Parkinsonia aculeata</t>
+  </si>
+  <si>
+    <t>Palo verde</t>
+  </si>
+  <si>
+    <t>Gregg's mistflower</t>
+  </si>
+  <si>
+    <t>Late boneset</t>
+  </si>
+  <si>
+    <t>Other boneset?</t>
+  </si>
+  <si>
+    <t>Lyreleaf sage</t>
+  </si>
+  <si>
+    <t>Ragweed</t>
+  </si>
+  <si>
+    <t>Inland sea oats</t>
+  </si>
+  <si>
+    <t>Golden groundsel</t>
+  </si>
+  <si>
+    <t>Illinois bundleflower</t>
+  </si>
+  <si>
+    <t>Desert mallow</t>
+  </si>
+  <si>
+    <t>Nuevo leon salvia</t>
+  </si>
+  <si>
+    <t>Elbow bush</t>
+  </si>
+  <si>
+    <t>Fall aster</t>
+  </si>
+  <si>
+    <t>Obedient plant</t>
+  </si>
+  <si>
+    <t>Skeleton leaf goldeneye</t>
+  </si>
+  <si>
+    <t>Cobweb spiderwort</t>
+  </si>
+  <si>
+    <t>Japanese thing near street</t>
+  </si>
+  <si>
+    <t>Pokeweed</t>
+  </si>
+  <si>
+    <t>Okra</t>
+  </si>
+  <si>
+    <t>American elm</t>
+  </si>
+  <si>
+    <t>Tree of heaven</t>
+  </si>
+  <si>
+    <t>Poison ?</t>
+  </si>
+  <si>
+    <t>Paw paw</t>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>Pumpkin</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>Horseweed</t>
+  </si>
+  <si>
+    <t>Standing cypress</t>
+  </si>
+  <si>
+    <t>Engelmann daisy</t>
+  </si>
+  <si>
+    <t>Dandelion</t>
+  </si>
+  <si>
+    <t>Milk thistle</t>
+  </si>
+  <si>
+    <t>Bramble thing</t>
+  </si>
+  <si>
+    <t>Black walnut?</t>
+  </si>
+  <si>
+    <t>Black hungarian pepper</t>
+  </si>
+  <si>
+    <t>Conoclinium greggii</t>
+  </si>
+  <si>
+    <t>Eupatorium serotinum</t>
+  </si>
+  <si>
+    <t>Salvia lyrata</t>
+  </si>
+  <si>
+    <t>Chasmanthium latifolium</t>
+  </si>
+  <si>
+    <t>Packera aurea</t>
+  </si>
+  <si>
+    <t>Dasmanthus illinoensis</t>
+  </si>
+  <si>
+    <t>Sphaeralcea ambigua</t>
+  </si>
+  <si>
+    <t>Salvia cohuilensis</t>
+  </si>
+  <si>
+    <t>Forestiera pubescens</t>
+  </si>
+  <si>
+    <t>Symphyotrichum cordifolium</t>
+  </si>
+  <si>
+    <t>Physostegia virginiana</t>
+  </si>
+  <si>
+    <t>Viguiera stenoloba</t>
+  </si>
+  <si>
+    <t>Tradescantia sillamontana</t>
+  </si>
+  <si>
+    <t>Phytolacca americana</t>
+  </si>
+  <si>
+    <t>Abelmoschus esculentus</t>
+  </si>
+  <si>
+    <t>Ulmus americana</t>
+  </si>
+  <si>
+    <t>Ailanthus altissima</t>
+  </si>
+  <si>
+    <t>Asimina triloba</t>
+  </si>
+  <si>
+    <t>Solanum lycopersicum</t>
+  </si>
+  <si>
+    <t>Solanum tuberosum</t>
+  </si>
+  <si>
+    <t>Erigeron canadensis</t>
+  </si>
+  <si>
+    <t>Engelmannia peristenia</t>
+  </si>
+  <si>
+    <t>Wood sorrel</t>
+  </si>
+  <si>
+    <t>Martha Gonzales rose</t>
+  </si>
+  <si>
+    <t>Rosa Martha Gonzales</t>
+  </si>
+  <si>
+    <t>Baldwins ironweed</t>
+  </si>
+  <si>
+    <t>Nut sedge</t>
+  </si>
+  <si>
+    <t>Western primrose?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="31">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2132,6 +2476,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF202122"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF474747"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -2220,7 +2612,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2274,22 +2666,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2612,20 +2999,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E7D2DB-E867-1641-9FC0-DC5B101B27EB}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" style="46" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5" style="47" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="48"/>
-    <col min="5" max="5" width="13.5" style="48" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="48"/>
+    <col min="1" max="1" width="28.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5" style="4" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="46"/>
+    <col min="5" max="5" width="13.5" style="46" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="46" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="46"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2649,1134 +3036,1757 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E2" s="48">
+      <c r="E2" s="46">
         <v>2022</v>
       </c>
-      <c r="F2" s="48">
+      <c r="F2" s="46">
         <v>2023</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="46" t="s">
         <v>573</v>
       </c>
-      <c r="E3" s="56">
+      <c r="E3" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" customHeight="1">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E4" s="56">
+      <c r="E4" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="46" t="s">
         <v>573</v>
       </c>
-      <c r="E5" s="56">
+      <c r="E5" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="7" t="s">
         <v>582</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E6" s="56">
+      <c r="E6" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="46" t="s">
         <v>573</v>
       </c>
-      <c r="E7" s="56">
+      <c r="E7" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E8" s="56">
+      <c r="E8" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E9" s="56">
+      <c r="E9" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E10" s="56">
+      <c r="E10" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E11" s="56">
+      <c r="E11" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E12" s="56">
+      <c r="E12" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="48" t="s">
+      <c r="B13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E13" s="56">
+      <c r="E13" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E14" s="56">
+      <c r="E14" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E15" s="56">
+      <c r="E15" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D16" s="48" t="s">
+      <c r="D16" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E16" s="56">
+      <c r="E16" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E17" s="56">
+      <c r="E17" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="D18" s="46" t="s">
         <v>573</v>
       </c>
-      <c r="E18" s="56">
+      <c r="E18" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D19" s="48" t="s">
+      <c r="D19" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E19" s="56">
+      <c r="E19" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="E20" s="56">
+      <c r="E20" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D21" s="48" t="s">
+      <c r="D21" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E21" s="56">
+      <c r="E21" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="48" t="s">
+      <c r="C22" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D22" s="48" t="s">
+      <c r="D22" s="46" t="s">
         <v>573</v>
       </c>
-      <c r="E22" s="56">
+      <c r="E22" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="C23" s="48" t="s">
+      <c r="C23" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D23" s="48" t="s">
+      <c r="D23" s="46" t="s">
         <v>573</v>
       </c>
-      <c r="E23" s="56">
+      <c r="E23" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D24" s="48" t="s">
+      <c r="D24" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E24" s="56">
+      <c r="E24" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="C25" s="48" t="s">
+      <c r="C25" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D25" s="48" t="s">
+      <c r="D25" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E25" s="56">
+      <c r="E25" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C26" s="48" t="s">
+      <c r="C26" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D26" s="48" t="s">
+      <c r="D26" s="46" t="s">
         <v>573</v>
       </c>
-      <c r="E26" s="56">
+      <c r="E26" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C27" s="48" t="s">
+      <c r="C27" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D27" s="48" t="s">
+      <c r="D27" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="F27" s="48">
+      <c r="F27" s="46">
         <v>2024</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D28" s="48" t="s">
+      <c r="D28" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E28" s="56">
+      <c r="E28" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="C29" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D29" s="48" t="s">
+      <c r="D29" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E29" s="56">
+      <c r="E29" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D30" s="48" t="s">
+      <c r="D30" s="46" t="s">
         <v>573</v>
       </c>
-      <c r="E30" s="56">
+      <c r="E30" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="48" t="s">
+      <c r="C31" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D31" s="48" t="s">
+      <c r="D31" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E31" s="56">
+      <c r="E31" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="50" t="s">
+      <c r="A32" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="C32" s="48" t="s">
+      <c r="C32" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D32" s="48" t="s">
+      <c r="D32" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E32" s="56">
+      <c r="E32" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="C33" s="48" t="s">
+      <c r="C33" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D33" s="48" t="s">
+      <c r="D33" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E33" s="56">
+      <c r="E33" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="50" t="s">
+      <c r="A34" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="4" t="s">
         <v>470</v>
       </c>
-      <c r="C34" s="48" t="s">
+      <c r="C34" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D34" s="48" t="s">
+      <c r="D34" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E34" s="56">
+      <c r="E34" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C35" s="48" t="s">
+      <c r="C35" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D35" s="48" t="s">
+      <c r="D35" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E35" s="56">
+      <c r="E35" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="48" t="s">
+      <c r="C36" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D36" s="48" t="s">
+      <c r="D36" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E36" s="56">
+      <c r="E36" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="46" t="s">
+      <c r="A37" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="C37" s="48" t="s">
+      <c r="C37" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D37" s="48" t="s">
+      <c r="D37" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E37" s="56">
+      <c r="E37" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="46" t="s">
+      <c r="A38" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="48" t="s">
+      <c r="C38" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D38" s="48" t="s">
+      <c r="D38" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E38" s="56">
+      <c r="E38" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="B39" s="47" t="s">
+      <c r="B39" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C39" s="48" t="s">
+      <c r="C39" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E39" s="56">
+      <c r="E39" s="47">
         <v>45511</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="51" t="s">
+        <v>652</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="C40" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D40" s="46" t="s">
+        <v>574</v>
+      </c>
+      <c r="E40" s="47">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="5" t="s">
         <v>482</v>
       </c>
-      <c r="B40" s="47" t="s">
+      <c r="B41" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="C40" s="48" t="s">
+      <c r="C41" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D40" s="48" t="s">
+      <c r="D41" s="46" t="s">
         <v>573</v>
       </c>
-      <c r="E40" s="56">
+      <c r="E41" s="47">
         <v>45511</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="46" t="s">
+    <row r="42" spans="1:6">
+      <c r="A42" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="B41" s="47" t="s">
+      <c r="B42" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="C41" s="48" t="s">
+      <c r="C42" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D41" s="48" t="s">
+      <c r="D42" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E41" s="56"/>
-      <c r="F41" s="48">
+      <c r="E42" s="47"/>
+      <c r="F42" s="46">
         <v>2024</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="46" t="s">
+    <row r="43" spans="1:6">
+      <c r="A43" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="B42" s="47" t="s">
+      <c r="B43" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C42" s="48" t="s">
+      <c r="C43" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D42" s="48" t="s">
+      <c r="D43" s="46" t="s">
         <v>573</v>
       </c>
-      <c r="E42" s="56">
+      <c r="E43" s="47">
         <v>45511</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="46" t="s">
+    <row r="44" spans="1:6">
+      <c r="A44" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="B43" s="47" t="s">
+      <c r="B44" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="C43" s="48" t="s">
+      <c r="C44" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D43" s="48" t="s">
+      <c r="D44" s="46" t="s">
         <v>573</v>
       </c>
-      <c r="E43" s="56">
+      <c r="E44" s="47">
         <v>45511</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="46" t="s">
+    <row r="45" spans="1:6">
+      <c r="A45" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B44" s="47" t="s">
+      <c r="B45" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C44" s="48" t="s">
+      <c r="C45" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D44" s="48" t="s">
+      <c r="D45" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E44" s="56">
+      <c r="E45" s="47">
         <v>45511</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="46" t="s">
+    <row r="46" spans="1:6">
+      <c r="A46" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="B45" s="47" t="s">
+      <c r="B46" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="C45" s="48" t="s">
+      <c r="C46" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D45" s="48" t="s">
+      <c r="D46" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E45" s="56">
+      <c r="E46" s="47">
         <v>45511</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="46" t="s">
+    <row r="47" spans="1:6">
+      <c r="A47" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="B46" s="47" t="s">
+      <c r="B47" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="C46" s="48" t="s">
+      <c r="C47" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D46" s="48" t="s">
+      <c r="D47" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E46" s="56">
+      <c r="E47" s="47">
         <v>45511</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="51" t="s">
+    <row r="48" spans="1:6">
+      <c r="A48" s="48" t="s">
         <v>583</v>
       </c>
-      <c r="B47" s="47" t="s">
+      <c r="B48" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="C47" s="48" t="s">
+      <c r="C48" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D47" s="48" t="s">
+      <c r="D48" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E47" s="56">
+      <c r="E48" s="47">
         <v>45511</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="46" t="s">
+    <row r="49" spans="1:6">
+      <c r="A49" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="B48" s="47" t="s">
+      <c r="B49" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C48" s="48" t="s">
+      <c r="C49" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D48" s="48" t="s">
+      <c r="D49" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E48" s="56">
+      <c r="E49" s="47">
         <v>44084</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="46" t="s">
+    <row r="50" spans="1:6">
+      <c r="A50" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="B49" s="47" t="s">
+      <c r="B50" s="4" t="s">
         <v>576</v>
       </c>
-      <c r="C49" s="48" t="s">
+      <c r="C50" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D49" s="48" t="s">
+      <c r="D50" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E49" s="56">
+      <c r="E50" s="47">
         <v>45511</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="46" t="s">
+    <row r="51" spans="1:6">
+      <c r="A51" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="B50" s="47" t="s">
+      <c r="B51" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="C50" s="48" t="s">
+      <c r="C51" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D50" s="48" t="s">
+      <c r="D51" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E50" s="56"/>
-      <c r="F50" s="48">
+      <c r="E51" s="47"/>
+      <c r="F51" s="46">
         <v>2023</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="46" t="s">
+    <row r="52" spans="1:6">
+      <c r="A52" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="B51" s="47" t="s">
+      <c r="B52" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="C51" s="48" t="s">
+      <c r="C52" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D51" s="48" t="s">
+      <c r="D52" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E51" s="56">
+      <c r="E52" s="47">
         <v>45511</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="46" t="s">
+    <row r="53" spans="1:6">
+      <c r="A53" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="B52" s="47" t="s">
+      <c r="B53" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="C52" s="48" t="s">
+      <c r="C53" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D52" s="48" t="s">
+      <c r="D53" s="46" t="s">
         <v>577</v>
       </c>
-      <c r="E52" s="56">
+      <c r="E53" s="47"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C54" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D54" s="46" t="s">
+        <v>574</v>
+      </c>
+      <c r="E54" s="47">
         <v>45511</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="46" t="s">
-        <v>302</v>
-      </c>
-      <c r="B53" s="47" t="s">
-        <v>300</v>
-      </c>
-      <c r="C53" s="48" t="s">
+    <row r="55" spans="1:6">
+      <c r="A55" s="49" t="s">
+        <v>519</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="C55" s="46" t="s">
+        <v>578</v>
+      </c>
+      <c r="D55" s="46" t="s">
+        <v>587</v>
+      </c>
+      <c r="E55" s="47">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="B56" s="34" t="s">
+        <v>554</v>
+      </c>
+      <c r="C56" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D53" s="48" t="s">
+      <c r="D56" s="46" t="s">
+        <v>575</v>
+      </c>
+      <c r="E56" s="47">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="B57" s="34" t="s">
+        <v>555</v>
+      </c>
+      <c r="C57" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D57" s="46" t="s">
+        <v>575</v>
+      </c>
+      <c r="E57" s="47">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="B58" s="34" t="s">
+        <v>556</v>
+      </c>
+      <c r="C58" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D58" s="46" t="s">
+        <v>573</v>
+      </c>
+      <c r="E58" s="47">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="49" t="s">
+        <v>559</v>
+      </c>
+      <c r="B59" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="C59" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D59" s="46" t="s">
+        <v>577</v>
+      </c>
+      <c r="E59" s="47">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="C60" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D60" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E53" s="56">
-        <v>45511</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="52" t="s">
-        <v>519</v>
-      </c>
-      <c r="B54" s="47" t="s">
-        <v>515</v>
-      </c>
-      <c r="C54" s="48" t="s">
+      <c r="E60" s="47">
+        <v>44085</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="50" t="s">
+        <v>603</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="C61" s="46" t="s">
         <v>578</v>
       </c>
-      <c r="D54" s="48" t="s">
+      <c r="D61" s="46" t="s">
         <v>587</v>
       </c>
-      <c r="E54" s="56">
-        <v>45511</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="53" t="s">
-        <v>581</v>
-      </c>
-      <c r="B55" s="54" t="s">
-        <v>554</v>
-      </c>
-      <c r="C55" s="48" t="s">
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="C62" s="46" t="s">
+        <v>578</v>
+      </c>
+      <c r="D62" s="46" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="C63" s="46" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="51" t="s">
+        <v>605</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="C64" s="46" t="s">
+        <v>578</v>
+      </c>
+      <c r="D64" s="46" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="C65" s="46" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="C66" s="46" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="C67" s="46" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="51" t="s">
+        <v>609</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="C68" s="46" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="C69" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D55" s="48" t="s">
+      <c r="D69" s="46" t="s">
+        <v>574</v>
+      </c>
+      <c r="E69" s="47">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="B70" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="C70" s="46" t="s">
+        <v>578</v>
+      </c>
+      <c r="D70" s="46" t="s">
+        <v>574</v>
+      </c>
+      <c r="E70" s="47">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="B71" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="C71" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D71" s="46" t="s">
+        <v>574</v>
+      </c>
+      <c r="E71" s="47">
+        <v>43950</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="C72" s="46" t="s">
+        <v>578</v>
+      </c>
+      <c r="D72" s="46" t="s">
+        <v>587</v>
+      </c>
+      <c r="E72" s="47">
+        <v>44085</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="5" t="s">
+        <v>611</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="C73" s="46" t="s">
+        <v>578</v>
+      </c>
+      <c r="D73" s="46" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="C74" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D74" s="46" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="5" t="s">
+        <v>615</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="C75" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D75" s="46" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="51" t="s">
+        <v>625</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="C76" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D76" s="46" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="C77" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D77" s="46" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="7" t="s">
+        <v>624</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="C78" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D78" s="46" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="5" t="s">
+        <v>622</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="C79" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D79" s="46" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="5" t="s">
+        <v>627</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="C80" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D80" s="46" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C81" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D81" s="46" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="51" t="s">
+        <v>629</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="C82" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D82" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E55" s="56">
-        <v>45511</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="53" t="s">
-        <v>580</v>
-      </c>
-      <c r="B56" s="54" t="s">
-        <v>555</v>
-      </c>
-      <c r="C56" s="48" t="s">
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="52" t="s">
+        <v>630</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>620</v>
+      </c>
+      <c r="C83" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D56" s="48" t="s">
+      <c r="D83" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E56" s="56">
-        <v>45511</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="53" t="s">
-        <v>579</v>
-      </c>
-      <c r="B57" s="54" t="s">
-        <v>556</v>
-      </c>
-      <c r="C57" s="48" t="s">
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="C84" s="46" t="s">
+        <v>645</v>
+      </c>
+      <c r="D84" s="46" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="C85" s="46" t="s">
+        <v>578</v>
+      </c>
+      <c r="D85" s="46" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="5" t="s">
+        <v>632</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>631</v>
+      </c>
+      <c r="C86" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D57" s="48" t="s">
+      <c r="D86" s="46" t="s">
         <v>573</v>
       </c>
-      <c r="E57" s="56">
-        <v>45511</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="55" t="s">
-        <v>559</v>
-      </c>
-      <c r="B58" s="54" t="s">
-        <v>558</v>
-      </c>
-      <c r="C58" s="48" t="s">
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="C87" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D58" s="48" t="s">
-        <v>577</v>
-      </c>
-      <c r="E58" s="56">
-        <v>45511</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="46" t="s">
-        <v>307</v>
-      </c>
-      <c r="B59" s="47" t="s">
-        <v>586</v>
-      </c>
-      <c r="C59" s="48" t="s">
+      <c r="D87" s="46" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>635</v>
+      </c>
+      <c r="C88" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D59" s="48" t="s">
+      <c r="D88" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E59" s="56">
-        <v>44085</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="B60" s="47" t="s">
-        <v>588</v>
-      </c>
-      <c r="C60" s="48" t="s">
-        <v>578</v>
-      </c>
-      <c r="D60" s="48" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="46" t="s">
-        <v>589</v>
-      </c>
-      <c r="B61" s="47" t="s">
-        <v>590</v>
-      </c>
-      <c r="C61" s="48" t="s">
-        <v>578</v>
-      </c>
-      <c r="D61" s="48" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="B62" s="47" t="s">
-        <v>591</v>
-      </c>
-      <c r="C62" s="48" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="B63" s="47" t="s">
-        <v>592</v>
-      </c>
-      <c r="C63" s="48" t="s">
-        <v>578</v>
-      </c>
-      <c r="D63" s="48" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="B64" s="47" t="s">
-        <v>594</v>
-      </c>
-      <c r="C64" s="48" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="B65" s="47" t="s">
-        <v>593</v>
-      </c>
-      <c r="C65" s="48" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="B66" s="47" t="s">
-        <v>595</v>
-      </c>
-      <c r="C66" s="48" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="B67" s="47" t="s">
-        <v>596</v>
-      </c>
-      <c r="C67" s="48" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="46" t="s">
-        <v>598</v>
-      </c>
-      <c r="B68" s="47" t="s">
-        <v>597</v>
-      </c>
-      <c r="C68" s="48" t="s">
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="7" t="s">
+        <v>640</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>637</v>
+      </c>
+      <c r="C89" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D68" s="48" t="s">
+      <c r="D89" s="46" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="C90" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D90" s="46" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="51" t="s">
+        <v>641</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>642</v>
+      </c>
+      <c r="C91" s="46" t="s">
+        <v>645</v>
+      </c>
+      <c r="D91" s="46" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="5" t="s">
+        <v>644</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="C92" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D92" s="46" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="5" t="s">
+        <v>646</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>647</v>
+      </c>
+      <c r="C93" s="46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D93" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="E68" s="56">
-        <v>44084</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="B69" s="47" t="s">
-        <v>599</v>
-      </c>
-      <c r="C69" s="48" t="s">
-        <v>578</v>
-      </c>
-      <c r="D69" s="48" t="s">
-        <v>574</v>
-      </c>
-      <c r="E69" s="56">
-        <v>44084</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="B70" s="47" t="s">
-        <v>600</v>
-      </c>
-      <c r="C70" s="48" t="s">
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="5" t="s">
+        <v>648</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="C94" s="46" t="s">
+        <v>645</v>
+      </c>
+      <c r="D94" s="46" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="C95" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="D70" s="48" t="s">
-        <v>574</v>
-      </c>
-      <c r="E70" s="56">
-        <v>43950</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="46" t="s">
-        <v>602</v>
-      </c>
-      <c r="B71" s="47" t="s">
-        <v>601</v>
-      </c>
-      <c r="C71" s="48" t="s">
-        <v>578</v>
-      </c>
-      <c r="D71" s="48" t="s">
-        <v>587</v>
-      </c>
-      <c r="E71" s="56">
-        <v>44085</v>
+      <c r="D95" s="46" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="B98" s="4" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="B100" s="4" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="5" t="s">
+        <v>694</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="5" t="s">
+        <v>697</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="51" t="s">
+        <v>699</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="7" t="s">
+        <v>700</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="53" t="s">
+        <v>702</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="B111" s="4" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="51" t="s">
+        <v>704</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="51" t="s">
+        <v>705</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="52" t="s">
+        <v>706</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="B117" s="4" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="51" t="s">
+        <v>707</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="51" t="s">
+        <v>708</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="B121" s="4" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="51" t="s">
+        <v>709</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="52" t="s">
+        <v>710</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="B126" s="4" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="B127" s="4" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="B128" s="4" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="B129" s="4" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="B130" s="4" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="B131" s="4" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="B134" s="4" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="B135" s="4" t="s">
+        <v>717</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F150">
-    <sortCondition ref="E2:E150"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F151">
+    <sortCondition ref="E2:E151"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3787,7 +4797,7 @@
   <dimension ref="A1:AB150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11028,23 +12038,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3B3D86-74ED-5D47-AE43-E8640BC5507C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8825AA-A5AA-EB48-96DA-617D57988EAB}">
   <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11727,11 +12725,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EDFA09-D8E2-6945-85F6-1E364B2A7A97}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>